<commit_message>
Định nghĩ các hàm trong solution Rest API
</commit_message>
<xml_diff>
--- a/Document/Định nghĩa hàm trong RestAPI.xlsx
+++ b/Document/Định nghĩa hàm trong RestAPI.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="124">
   <si>
     <t>Class</t>
   </si>
@@ -25,18 +25,12 @@
     <t>Mô tả</t>
   </si>
   <si>
-    <t>param</t>
-  </si>
-  <si>
     <t>Kết quả trả về</t>
   </si>
   <si>
     <t>ChiNhanhNHLogic.cs</t>
   </si>
   <si>
-    <t>DANH SÁCH CÁC HÀM ĐƯỢC ĐỊNH NGHĨA TẠI RESTAPI</t>
-  </si>
-  <si>
     <t>CTGiaoDichLogic.cs</t>
   </si>
   <si>
@@ -62,13 +56,345 @@
   </si>
   <si>
     <t>RestAPILogic.cs</t>
+  </si>
+  <si>
+    <t>RestAPILogic.cs là class chứa các logic có nghiệp vụ đặc biệt.
+Trường hợp cần add thêm method nào thì hãy điền rõ các thông tin trên và tô background color là màu vàng, khi tôi hoàn thành sẽ setting background color là None</t>
+  </si>
+  <si>
+    <t>SearchAllBankBranches()</t>
+  </si>
+  <si>
+    <t>List&lt;ChiNhanhNganHang&gt;</t>
+  </si>
+  <si>
+    <t>Lấy tất cả các Chi nhánh ngân hàng</t>
+  </si>
+  <si>
+    <t>SearchBankBranchesByCondition</t>
+  </si>
+  <si>
+    <t>ChiNhanhNganHang sc</t>
+  </si>
+  <si>
+    <t>Lấy danh sách chi nhánh với param là model ChiNhanhNganHang</t>
+  </si>
+  <si>
+    <t>InsertBankBranches</t>
+  </si>
+  <si>
+    <t>ChiNhanhNganHang objInsert</t>
+  </si>
+  <si>
+    <t>UpdateBankBranches</t>
+  </si>
+  <si>
+    <t>ChiNhanhNganHang objUpdate</t>
+  </si>
+  <si>
+    <t>Insert đối tượng vào DB</t>
+  </si>
+  <si>
+    <t>Update đối tượng vào DB</t>
+  </si>
+  <si>
+    <t>DeleteBankBranches</t>
+  </si>
+  <si>
+    <t>List&lt;string&gt; lstID (với lstID là list các MaCN muốn xóa khỏi DB)</t>
+  </si>
+  <si>
+    <t>DANH SÁCH CÁC HÀM ĐƯỢC ĐỊNH NGHĨA TẠI REST API</t>
+  </si>
+  <si>
+    <t>SearchAllDealDetail()</t>
+  </si>
+  <si>
+    <t>List&lt;ChiTietGiaoDich&gt;</t>
+  </si>
+  <si>
+    <t>Lấy tất cả các chi tiết giao dịch</t>
+  </si>
+  <si>
+    <t>Lấy tất cả các chi tiết giao dịch với param là model ChiTietGiaoDich</t>
+  </si>
+  <si>
+    <t>SearchDealDetailByCondition</t>
+  </si>
+  <si>
+    <t>ChiTietGiaoDich sc</t>
+  </si>
+  <si>
+    <t>InsertDealDetail</t>
+  </si>
+  <si>
+    <t>UpdateDealDetail</t>
+  </si>
+  <si>
+    <t>DeleteDealDetail</t>
+  </si>
+  <si>
+    <t>DeleteDeal</t>
+  </si>
+  <si>
+    <t>UpdateDeal</t>
+  </si>
+  <si>
+    <t>InsertDeal</t>
+  </si>
+  <si>
+    <t>SearchAllDeal</t>
+  </si>
+  <si>
+    <t>Delete đối tượng ra khỏi DB</t>
+  </si>
+  <si>
+    <t>ChiTietGiaoDich objInsert</t>
+  </si>
+  <si>
+    <t>ChiTietGiaoDich objUpdate</t>
+  </si>
+  <si>
+    <t>List&lt;ChiTietGiaoDich&gt; lstID</t>
+  </si>
+  <si>
+    <t>Lấy tất cả các giao dịch</t>
+  </si>
+  <si>
+    <t>GiaoDich sc</t>
+  </si>
+  <si>
+    <t>List&lt;GiaoDich&gt;</t>
+  </si>
+  <si>
+    <t>GiaoDich objInsert</t>
+  </si>
+  <si>
+    <t>GiaoDich objUpdate</t>
+  </si>
+  <si>
+    <t>List&lt;string&gt; lstID</t>
+  </si>
+  <si>
+    <t>InsertCustomer</t>
+  </si>
+  <si>
+    <t>UpdateCustomer</t>
+  </si>
+  <si>
+    <t>DeleteCustomer</t>
+  </si>
+  <si>
+    <t>SearchAllCustomer</t>
+  </si>
+  <si>
+    <t>SearchCustomerByCondition</t>
+  </si>
+  <si>
+    <t>Lấy tất cả danh sách khách hàng</t>
+  </si>
+  <si>
+    <t>Lấy danh sách khách hàng với param là model KhachHang</t>
+  </si>
+  <si>
+    <t>Lấy danh sách chi nhánh với param là model GiaoDich</t>
+  </si>
+  <si>
+    <t>List&lt;KhachHang&gt;</t>
+  </si>
+  <si>
+    <t>KhachHang sc</t>
+  </si>
+  <si>
+    <t>KhachHang customer</t>
+  </si>
+  <si>
+    <t>List&lt;string&gt; lstKH</t>
+  </si>
+  <si>
+    <t>SearchAllBanking</t>
+  </si>
+  <si>
+    <t>SearchBankingByCondition</t>
+  </si>
+  <si>
+    <t>Lấy danh sách ngân hàng với param là model NganHang</t>
+  </si>
+  <si>
+    <t>Lấy tất cả các ngân hàng</t>
+  </si>
+  <si>
+    <t>InsertBanking</t>
+  </si>
+  <si>
+    <t>List&lt;NganHang&gt;</t>
+  </si>
+  <si>
+    <t>NganHang sc</t>
+  </si>
+  <si>
+    <t>UpdateBanking</t>
+  </si>
+  <si>
+    <t>NganHang objUpdate</t>
+  </si>
+  <si>
+    <t>NganHang objInsert</t>
+  </si>
+  <si>
+    <t>DeleteBanking</t>
+  </si>
+  <si>
+    <t>SearchAllStaff</t>
+  </si>
+  <si>
+    <t>SearchStaffByCondition</t>
+  </si>
+  <si>
+    <t>List&lt;NhanVien&gt;</t>
+  </si>
+  <si>
+    <t>NhanVien sc</t>
+  </si>
+  <si>
+    <t>InsertStaff</t>
+  </si>
+  <si>
+    <t>Lấy cả các nhân viên</t>
+  </si>
+  <si>
+    <t>Lấy danh sách nhân viên với param là model NhanVien</t>
+  </si>
+  <si>
+    <t>NhanVien staff</t>
+  </si>
+  <si>
+    <t>UpdateStaff</t>
+  </si>
+  <si>
+    <t>DeleteStaff</t>
+  </si>
+  <si>
+    <t>List&lt;string&gt; lstMaNV</t>
+  </si>
+  <si>
+    <t>SearchAllSaveMoney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List&lt;SoTietKiem&gt; </t>
+  </si>
+  <si>
+    <t>Lấy tất cả thông tin sổ tiết kiệm</t>
+  </si>
+  <si>
+    <t>Lấy thông tin sổ tiết kiệm với param là model SoTietKiem</t>
+  </si>
+  <si>
+    <t>SearchSaveMoneyByCondition</t>
+  </si>
+  <si>
+    <t>SoTietKiem sc</t>
+  </si>
+  <si>
+    <t>InsertSaveMoney</t>
+  </si>
+  <si>
+    <t>SoTietKiem objInsert</t>
+  </si>
+  <si>
+    <t>UpdateSaveMoney</t>
+  </si>
+  <si>
+    <t>SoTietKiem objUpdate</t>
+  </si>
+  <si>
+    <t>DeleteSaveMoney</t>
+  </si>
+  <si>
+    <t>List&lt;SoTietKiem&gt; lstID</t>
+  </si>
+  <si>
+    <t>SearchAllAccount</t>
+  </si>
+  <si>
+    <t>List&lt;TaiKhoan&gt;</t>
+  </si>
+  <si>
+    <t>Lấy tất cả thông tin về tài khoản</t>
+  </si>
+  <si>
+    <t>SearchAccountByCondition</t>
+  </si>
+  <si>
+    <t>TaiKhoan sc</t>
+  </si>
+  <si>
+    <t>Lấy thông tin tài khoản với param là model TaiKhoan</t>
+  </si>
+  <si>
+    <t>InsertAccount</t>
+  </si>
+  <si>
+    <t>TaiKhoan objInsert</t>
+  </si>
+  <si>
+    <t>UpdateAccount</t>
+  </si>
+  <si>
+    <t>TaiKhoan objUpdate</t>
+  </si>
+  <si>
+    <t>DeleteAccount</t>
+  </si>
+  <si>
+    <t>List&lt;TaiKhoan&gt; lstID</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>CheckLogin</t>
+  </si>
+  <si>
+    <t>Lấy thông tin nhân viên dựa vào userid và password đăng nhập. Mặc định userid chính là MaNV của NhanVien</t>
+  </si>
+  <si>
+    <t>string userId,
+string pass</t>
+  </si>
+  <si>
+    <t>model NhanVien</t>
+  </si>
+  <si>
+    <t>InsertUser</t>
+  </si>
+  <si>
+    <t>Thêm 1 user mới</t>
+  </si>
+  <si>
+    <t>MSTUSER objInsert</t>
+  </si>
+  <si>
+    <t>UpdateUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cập nhật thông tin user </t>
+  </si>
+  <si>
+    <t>MSTUSER objUpdate</t>
+  </si>
+  <si>
+    <t>DeleteUser</t>
+  </si>
+  <si>
+    <t>Delete 1 user. Cách delete ở đây là setting flag DELETE_YMD = Date.Now là được. Lúc CheckLogin chỉ thỏa khi DELETE_YMD  == NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +427,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -116,7 +449,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -418,11 +751,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -434,10 +820,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,20 +835,65 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,10 +1199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F57"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -783,7 +1211,7 @@
     <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40" style="3" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="41.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="45.5703125" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1" hidden="1"/>
@@ -791,11 +1219,11 @@
   <sheetData>
     <row r="1" spans="2:6" ht="18" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
-      <c r="C1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="C1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -806,424 +1234,744 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="21" t="s">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
+      <c r="C4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="25"/>
+      <c r="C5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="25"/>
+      <c r="C6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="25"/>
+      <c r="C7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="2:6" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B8" s="25"/>
+      <c r="C8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="24"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="24"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="24"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="24"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="25" t="s">
+      <c r="C9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="25"/>
+      <c r="C10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="25"/>
+      <c r="C11" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="25"/>
+      <c r="C12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="26"/>
+      <c r="C13" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B15" s="25"/>
+      <c r="C15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="25"/>
+      <c r="C16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="25"/>
+      <c r="C17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="26"/>
+      <c r="C18" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="24"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="24"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="24"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="26"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="25" t="s">
+      <c r="C19" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="25"/>
+      <c r="C20" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="25"/>
+      <c r="C21" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="25"/>
+      <c r="C22" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B23" s="26"/>
+      <c r="C23" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="24"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="24"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="26"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="25" t="s">
+      <c r="C24" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B25" s="25"/>
+      <c r="C25" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="25"/>
+      <c r="C26" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="25"/>
+      <c r="C27" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="21"/>
+    </row>
+    <row r="28" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="26"/>
+      <c r="C28" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="24"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="24"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="24"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="26"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="25" t="s">
+      <c r="C29" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B30" s="25"/>
+      <c r="C30" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="25"/>
+      <c r="C31" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="25"/>
+      <c r="C32" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="21"/>
+    </row>
+    <row r="33" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="26"/>
+      <c r="C33" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="23"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="24"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="24"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="24"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="26"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="25" t="s">
+      <c r="C34" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B35" s="25"/>
+      <c r="C35" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="25"/>
+      <c r="C36" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="25"/>
+      <c r="C37" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="21"/>
+    </row>
+    <row r="38" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="26"/>
+      <c r="C38" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="23"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="24"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="24"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="24"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="26"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="25" t="s">
+      <c r="C39" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B40" s="25"/>
+      <c r="C40" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="25"/>
+      <c r="C41" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" s="21"/>
+    </row>
+    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="25"/>
+      <c r="C42" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="26"/>
+      <c r="C43" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B44" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="24"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="24"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="24"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="26"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="25" t="s">
+      <c r="C44" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="25"/>
+      <c r="C45" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="21"/>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="25"/>
+      <c r="C46" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="21"/>
+    </row>
+    <row r="47" spans="2:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B47" s="25"/>
+      <c r="C47" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="21"/>
+    </row>
+    <row r="48" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="26"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="23"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="24"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="24"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="24"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="26"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="14"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="25" t="s">
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="19"/>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="25"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="21"/>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="25"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="21"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="25"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="21"/>
+    </row>
+    <row r="53" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="26"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="23"/>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="24"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="7"/>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="24"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="24"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="26"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="12"/>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="24"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="24"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7"/>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="24"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="2:6" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="26"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
-    </row>
-    <row r="54" spans="2:6" s="3" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="16"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="18"/>
-    </row>
-    <row r="55" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="5"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="7"/>
-    </row>
-    <row r="56" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="5"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="7"/>
-    </row>
-    <row r="57" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="8"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="10"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="31"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="32"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="34"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="32"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="34"/>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="32"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="34"/>
+    </row>
+    <row r="58" spans="2:6" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="37"/>
+    </row>
+    <row r="59" spans="2:6" s="3" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="12"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="14"/>
+    </row>
+    <row r="60" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="5"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="8"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="B54:F58"/>
     <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B49:B53"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="B39:B43"/>
     <mergeCell ref="B44:B48"/>

</xml_diff>